<commit_message>
Some changes the code in prices
</commit_message>
<xml_diff>
--- a/MAKEMYTRIP/src/main/java/com/mmt/excel/randomradiobutton.xlsx
+++ b/MAKEMYTRIP/src/main/java/com/mmt/excel/randomradiobutton.xlsx
@@ -125,13 +125,13 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.47"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="14.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="25.06"/>
@@ -150,34 +150,34 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="0" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4" s="0" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="n">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Design doc file
</commit_message>
<xml_diff>
--- a/MAKEMYTRIP/src/main/java/com/mmt/excel/randomradiobutton.xlsx
+++ b/MAKEMYTRIP/src/main/java/com/mmt/excel/randomradiobutton.xlsx
@@ -122,7 +122,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
@@ -172,14 +172,6 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>